<commit_message>
Get daily reddit data: Tue Jul  9 08:08:14 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_14.xlsx
+++ b/data/2024_07_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C480"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3049 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1dyvyqt</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>This design &gt; obsessed!</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyvyqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1dyuyae</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>first time doing my own glue ons (painted on myself!)</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyuyae</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1dyum9p</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>MOONCAT - Arthemis' Deathkiss</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyum9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1dyucpe</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Gel X or builder gel?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyucpe/gel_x_or_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1dyuc68</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Flowers by me (excuse my cuticles i had an anxiety episo)</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyuc68</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1dyu2ji</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Full set price</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2yd314edfbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1dytiqy</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>What shape do you think would best suit this color</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dytiqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1dytdem</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>help me design my nails:)</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dytdem</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1dysosi</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>fun little set!</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dysosi</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1dysf1k</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Want to try a natural gel?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dysf1k/want_to_try_a_natural_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1dys7c6</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Olive and June nails are as advertised</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ubyy3nruebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1dys585</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">made especially for a rock concert </t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dys585</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1dyrwew</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Simple But Cute Set w My Boyfriend's Initials 🥰</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0k2ofoyrebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1dyru9u</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>I finally got to try cat eye nails and I love them!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/352n6txdrebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1dyrlsm</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Nail set my friend did for me</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujfkgcy5pebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1dyrkfq</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Posting this so I have motivation to STOP BITING omg</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyrkfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1dyrjqj</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Just got them done today....</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rabzcgkoebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1dyrds2</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>What is this bit for?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohf4krp1nebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1dyrgsv</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Was inspired by the nails u/gemiiniiviirgo did and now l'm obsessed with my nails!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyrgsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1dyrdun</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>can you get your nails soaked off anywhere?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyrdun/can_you_get_your_nails_soaked_off_anywhere/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1dyr96o</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shellac peeling off in 3-4 days </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyr96o/shellac_peeling_off_in_34_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1dyr3xr</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>My take on rose quartz…with a hint of gold.</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6pe3lhemkebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1dyqpmb</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>New glue on nails</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyqpmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1dymmk7</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>I am having decision paralysis</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dymmk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1dynp5h</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>It's nice but I'm unsure if I overpaid for it. How much do you think this cost?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jrvp8ewqdbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1dypdxh</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>My client’s birthday set 🔥🧊</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kpatp2w45ebd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1dypzvl</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>A word of caution to the press-on gals and guys</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dypzvl/a_word_of_caution_to_the_presson_gals_and_guys/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1dyq9so</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Couldn’t decide, so asked for both! </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyq9so</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1dyq266</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Can't get a KISS nail glue open</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyq266</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1dypwi5</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Getting back into it</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dypwi5</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1dyppl9</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is my nail shape good? </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyppl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1dypmvb</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Tried out press-ons for the first time ahead of my engagement photo shoot and wedding. I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvg4ezio7ebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1dyp2rw</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> CAnt go wrong with frenchies 💅💅💅💕💕💕</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ll7ututx2ebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1dyoyqc</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Square long, almond/round long, or round short? 💅🏻</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyoyqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1dyowr4</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>My take on fruit nails</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyowr4</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1dyow43</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>would you call this holographic? 🤔</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwtnfcad1ebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1dyno8g</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Blue chrome moment</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7aunn1ardbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1dynk00</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any guesses what movie this set I’m working on is from? </t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4t02zvcqdbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1dyn8gy</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Natural nail growth: best combination of products</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyn8gy/natural_nail_growth_best_combination_of_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1dympb6</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel manicure on natural nails. Im a recovering nail biter, ~8 months no biting! </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9px7726pjdbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1dymliw</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Newish to nails</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dymliw</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1dymk8l</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>How to execute these with gel?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1h3xsumidbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1dymcv4</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Tool to use instead of fingers as tools</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dymcv4/tool_to_use_instead_of_fingers_as_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1dym60a</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>OPI gel polish</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dym60a/opi_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1dym45e</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In what way do they fit me better? I read them </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dym45e</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1dylx3q</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Rough nail edge after manicure</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dylx3q/rough_nail_edge_after_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1dylgch</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>grunge 🤝🏻 coquette</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dylgch</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1dyjwrf</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Anyone else feels bad to ask their nail tech for designs?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyjwrf/anyone_else_feels_bad_to_ask_their_nail_tech_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1dyjuu6</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Is there a similar nail polish out there? (Nailwork not mine - Pic from Pinterest)</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtagut6uycbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1dyl3x9</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Apologies for low quality image. How can I fix this nail shape?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejky40gv7dbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1dykpyz</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>HELP! I Need Beginner's Guide to Nail Protection</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dykpyz/help_i_need_beginners_guide_to_nail_protection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1dykidg</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>What nail color would suit me</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lh3k4bi3dbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1dykd4q</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Sand and Beach</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dykd4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1dyjzto</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>From nail biter to mermaid princess</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyjzto</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1dyj3mn</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Some might say they’re extra but for me, they’re perfect</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gi0rn9vitcbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1dyipw6</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>can you use builder gel as glue for gel x?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyipw6/can_you_use_builder_gel_as_glue_for_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1dyipov</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Dent from Acrylics</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thrdyo1tqcbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1dyimu9</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>new set!</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyimu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1dyiixh</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Normal growth? A week and five days - first time I've gotten nails done</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyiixh</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1dyimgd</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>What shape would suit my short nail beds?</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bad489c5qcbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1dyih86</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Summer strawberries 🍓</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ab59zwe4pcbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1dyfv33</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Acrylic on bruised nail?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyfv33</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1dyflzq</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Anyone else?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyflzq/anyone_else/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1dyf4w4</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Should I redo my gel manicure early before a long trip?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qyrrgfk61cbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1dydkbp</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Can I please get some advice?</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dydkbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1dycmvy</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>rawrrrr 🐾</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dycmvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1dycczg</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Kiss press on nails</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dycczg/kiss_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1dyccru</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Helppp</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyccru</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1dyb4xl</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Sassy Saints - any reviews and color recommendations?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fapbwlm68bbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1dyarzi</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which bow design goes best with the nails? </t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyarzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1dy9ha3</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My clients nail is coming off </t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dy9ha3/my_clients_nail_is_coming_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1dy6x7v</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for Essence Space Queen</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dy6x7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1dy5yxq</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>What’s the least damaging way to do extensions?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dy5yxq/whats_the_least_damaging_way_to_do_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1dy3vyc</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Best adhesive for press ons?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dy3vyc/best_adhesive_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1dyico0</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Cute lil fish 🐟</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyico0</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1dy1exd</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Need advice on how could I communicate with my nail tech better.</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dy1exd/need_advice_on_how_could_i_communicate_with_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1dy17hd</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>My last 4 manicures</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dy17hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1dy0n4c</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trim cuticles or nah? </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dy0n4c/trim_cuticles_or_nah/</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1dygoyf</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Inspired by the eyes of my favorite cat</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/si2ftnd3ccbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1dygupg</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>what can i do differently?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dygupg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1dyh6jg</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>An eternity later , i present : my second time doing my nails at home</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyh6jg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1dyi7qt</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Why does my tacky layer not come off</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyi7qt/why_does_my_tacky_layer_not_come_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1dyhxek</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>1st time doing my own gel nails</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyhxek</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1dyhj68</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I’m basically in love with my new nails!</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw7dmim9icbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1dyhfil</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art novice </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hk16osnjhcbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1dyhdve</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>What color are these, exactly? 😏</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjjuif58hcbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1dyh9i3</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Perfect babyboomer, what do you think?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snqnr5ocgcbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1dyh44r</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>For any nail techs in this sub, are my nails too damaged to get them done (gel x)?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyh44r</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1dygoig</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>In love with the subtle shimmer tips</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dygoig</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1dygn62</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>I did my own nails for my wedding</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dygn62</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1dyghps</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Square/coffin vs Almond</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyghps</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1dyggb3</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Fill in I did on my client!</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxzo58skacbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1dygds0</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Gel glitter set from a few months ago ✨</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dygds0</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1dyepxt</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Press Ons</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyepxt/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1dyeplm</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Nail Growth</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyeplm/nail_growth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1dyejir</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Summer Vibes</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46u5rycwwbbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1dyedr0</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>I feel amazing in these 😩</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytjvss6qvbbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1dye4wr</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Question about curing glue under charms</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dye4wr/question_about_curing_glue_under_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1dyds0q</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Hello! Just shorted my nails down, what color do you guys Think Will suit me.</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mhhp58frbbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1dydjfb</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Letting my nails grow: Week 5</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13jo0dyqpbbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1dyuuzu</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Essie shade similar to Opi Lincoln Park After Dark?</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dyuuzu/essie_shade_similar_to_opi_lincoln_park_after_dark/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1dyusp7</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Using the heat to my advantage</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9xeihiy3lfbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1dyukzy</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>MOONCAT - Arthemis' Deathkiss</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyukzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1dyr27d</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Can anyone help?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xuwk1tb6kebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1dyt9a6</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>ILNP bottle lids getting sticky</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dyt9a6/ilnp_bottle_lids_getting_sticky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1dyl5vq</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Product recommendations?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zb7nmzc98dbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1dykycr</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Quick rainy day paint job</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dykycr</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1dyrw3u</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Why does ILNP Glass Candy get so goopy after a few uses?!? 😭😭</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dyrw3u/why_does_ilnp_glass_candy_get_so_goopy_after_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1dyrvpw</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>My first fancy gloss</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x94wv59rrebd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1dyq7et</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel removal: Is it okay to use a nail drill or is it damaging? </t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dyq7et/gel_removal_is_it_okay_to_use_a_nail_drill_or_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1dypids</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Loving this shine!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjinde7n6ebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1dyp3se</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Where does everyone get their polish??</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dyp3se/where_does_everyone_get_their_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1dyozpf</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Betsey Johnson</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyozpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1dyo8iu</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Summer can never last long enough ☀️</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyo8iu</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1dyng84</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>10/10 no notes ✨</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyng84</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1dymb4s</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Cirque Lucky Bag🍀</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dymb4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1dym0ro</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Finally tried layering and I’m obsessed with the results</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dym0ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1dylr5i</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>So what’s been going on with PPU?</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dylr5i/so_whats_been_going_on_with_ppu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1dylk86</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>How to get even coats for jelly polish?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dylk86</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1dyl2iw</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Greens! 💚</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyl2iw</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1dyk9zu</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>The many shades of Am I Everything You Fear</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyk9zu</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1dyjlny</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BOGO 50% Sale on several nail polish brands at Ulta thru 7/13 </t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dyjlny/bogo_50_sale_on_several_nail_polish_brands_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1dyiuzq</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Can I apply gel polish over Nailtiques?</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dyiuzq/can_i_apply_gel_polish_over_nailtiques/</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1dyibx9</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favourite Scented Topcoat? </t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dyibx9/favourite_scented_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1dyi5xq</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for an old NYC Polish [Times Square Tangerine Cream]</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.makeupalley.com/product/showreview.asp/ItemId=89438/Long-Wearing-Nail-Enamel---Times-Sq-Tangerine-112/NYC-New-York-Color/Polishes</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1dyi5gi</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Chipping in the same spot, is this bc of the apex?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfkge0msmcbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1dyi4ii</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>I love nail polish and I love Twin Peaks, so here’s my Diane manicure</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyi4ii</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1dyi2qn</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Unconventional plea for assistance</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6yfbxp8mcbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1dyi0g1</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Once in a blue moon, I gravitate towards this colour</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s13ylm1rlcbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1dyhj3m</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Forgot how pretty this one was</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kloqch39icbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1dygqe4</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Disappointed in Death Valley Nails</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dygqe4/disappointed_in_death_valley_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1dygdb3</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Summer fun! 🕶️☀️</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dygdb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1dyg72y</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Store open</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dyg72y/store_open/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1dyfv6h</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Take me to your later </t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upqvii8e6cbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1dxzplo</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>essie’s feelin’ just lime dupe?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dxzplo/essies_feelin_just_lime_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1dyf16k</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>🥭🥭🥭</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyf16k</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1dyf0js</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black jelly polish </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dyf0js/black_jelly_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1dyemnk</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Blossom's Breath over Treachery In The Blue</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dyemnk/blossoms_breath_over_treachery_in_the_blue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1dyegcz</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Hosted a nail painting party over the weekend, here is my new sparkle ✨️</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyegcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1dydzq6</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>BKL [redacted]</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dydzq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1dydfbs</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Base coat versus Topcoat: which is more important?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dydfbs/base_coat_versus_topcoat_which_is_more_important/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1dydeom</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>ILNP’s holos are no joke</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dydeom</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1dyd9vs</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Purple Marble Nails</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyd9vs</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1dyck28</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Grayscale skittle</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyck28</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1dycf9n</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Does anyone know any dupes for this blue from Madam Glam</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dycf9n/does_anyone_know_any_dupes_for_this_blue_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1dyanmf</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>such a fun set!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyanmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1dyagim</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>My first Drunk Fairy polish. So pretty! 🤩</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyagim</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1dy9dgl</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Cirque Colors Lucky Bag Swatches (forgive the mess lol)</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dy9dgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1dy9abq</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Looking for this Berry color?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lc06jpztabd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1dy93ww</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best / Favorite DVN shades? </t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dy93ww/best_favorite_dvn_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1dy8tzj</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails inc - Rising Sun Court </t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dy8tzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1dy8fps</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My jaw was on the floor when I started painting! </t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dy8fps</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1dy7wvl</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The depth of this polish. So shiny! </t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2b4jny3jiabd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1dy5v28</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Wanted dinosaur-skin nails for my kid’s birthday… dramatic photo shoot felt necessary.</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dy5v28</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1dy554f</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dy554f/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1dy4sqe</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Painted this on so sloppily before work bc I couldn't wait to try it but it still looks amazing😭❤️(thumb cencored bc it has a gross looking wound that ruins the vibe)</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dy4sqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1dys8pu</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Duck Nails</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dys8pu</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1dyrjo7</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>A detailed video on making nail art gel</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w5z5ab2joebd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1dyqsqf</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>trad ink set ❤️💎</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyqsqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1dypxb7</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>My first time nail stamping!</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/byi2alg6aebd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1dyltpw</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Nails of the day 🥵</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4zatg73ddbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1dyl1oj</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Did these yesterday, a little bumpy but I love them</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mc90yave7dbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1dyhpu1</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Red roses</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyhpu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1dygjby</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Flintstone Nails</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldqizl76bcbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1dyghbr</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>3D ladybird nails with encapsulated skeleton leaves - made for a Cottagecore themed market</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bciwsznracbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1dygew0</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Marble 💜</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1l6yhybaacbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1dygev4</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>What do you all think of this set I'm thinking of getting? Going to the beach soon and wanted something "beachy"</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tearte6aacbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1dygdbc</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>My last set two weeks ago.</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgkncrky9cbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1dyf2o0</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Toppers </t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dyf2o0/toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1dyf0c9</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Tried some subtle koi nails</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyf0c9</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1dyf07h</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Red and black dragon nails</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62rmq2z80cbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1dyeits</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Lavender Fields 💜</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/md1438drwbbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1dyeg4h</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Summer Vibes</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dquuurb7wbbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1dyd862</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French tips </t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyd862</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1dyd2jh</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Set of press ons I did for myself ✨</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyd2jh</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1dyadi0</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blooming/Tie Dye Gel X! </t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0993isgg2bbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1dy9zzc</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Chocolate tigers</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dy9zzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1dy8dn6</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Need some nail help!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m0ghcnimabd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1dy4xcs</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Took me 4 hours !!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dy4xcs</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jul 10 08:10:58 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_14.xlsx
+++ b/data/2024_07_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C480"/>
+  <dimension ref="A1:C652"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8593,6 +8593,2930 @@
         </is>
       </c>
     </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1dzp9wm</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t xml:space="preserve">marvel nails I did for my brother </t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzp9wm</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1dzp8bd</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why is it that when painting my natural nails with gel, without a base coat or prep, it doesn’t last, but when I paint fake nails with gel, (like gel X or polygel nails) it lasts? </t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dzp8bd/why_is_it_that_when_painting_my_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1dzp0fy</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>What do you think of my natural nails?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4vdj39zzmbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1dzotb1</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Chrome nails for $60</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0qiyzwpmxmbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1dzodal</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Help! I need pearl suggestions for wedding nails! 💅🏻</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udzwgl2lsmbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1dzns32</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>New set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzns32</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1dznkts</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Ombre Bandana 🌈</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyxp1ydojmbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1dzmurh</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>nail polish changed color after top coat?</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzmurh</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1dzmqta</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>where can i get a russian manicure and pedicure?</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dzmqta/where_can_i_get_a_russian_manicure_and_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1dzlazz</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Summer Vibes</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hq41pxc5xlbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1dzkq05</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>My new acrylics look off to me</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbd3hqwtrlbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1dzkrvx</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Need suggestions!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lg67f6bslbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1dzmc4h</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oo2dfmxx6mbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1dzlzw2</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Short n sweet</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2694bvo3mbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1dzlo6w</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Finished painting my bobs burgers nail set 🥰</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/866b7mwl0mbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1dzln4v</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>My friend has a nail charm that glows</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wa269vb0mbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1dzktsd</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Home-manicure</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8z8dkbpsslbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1dzktdw</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Did my own gelx nails for the first time!</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzktdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1dzknpn</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>New to nails</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dzknpn/new_to_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1dzknh6</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Pearl / X / Maxxxine set! Guess how long these took me 🤣</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/davsudh7rlbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1dzkh4s</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my own nails for my wedding on Saturday </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzkh4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1dzkfav</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>milky white shimmer topped with black flake taco</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzkfav</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1dzk051</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>I love my ducky</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhc9rf29llbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1dzjrsg</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Which shape suits my hands?</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzjrsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1dzijhf</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Insta recs for natural short nail inspiration?</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dzijhf/insta_recs_for_natural_short_nail_inspiration/</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1dzix4p</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Pink and short</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzix4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1dzivf1</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Pink sparkle</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b57k099fblbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1dziugi</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>fairly certain nails were done with MMA…</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dziugi/fairly_certain_nails_were_done_with_mma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1dzini5</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Non-gel cat eye polish recommendations</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dzini5/nongel_cat_eye_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1dzigf9</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Crying in bed because of HEMA allergy - positive comments please I’m terrified</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dzigf9/crying_in_bed_because_of_hema_allergy_positive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1dzi2xv</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Getting a little better each time!</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzi2xv</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1dzig9t</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Collection of sets I've had done!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzig9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1dziasf</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Bubbles in Nail Polish</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dziasf/bubbles_in_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1dziapo</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>This purple is EVERYTHING!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mdykn3j6lbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1dzi6sy</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails with my lil’ niece </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4v30ueim5lbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1dzi6j6</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pink or black? </t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b82nefvj5lbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1dzi0z6</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>DIY Nails 🖤</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzi0z6</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1dzhn3i</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Help! Is this the best shape for my nails?</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzhn3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1dzh39k</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Time for a refill!</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2pnmxelwkbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1dzgzg1</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Should I change nail shapes?</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzgzg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1dzfijn</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>How do I make my nails stronger?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dzfijn/how_do_i_make_my_nails_stronger/</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1dzgel6</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>41M - My very first pedi &amp; colour - so happy with them! (excuse clutter)</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynir7nqxqkbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1dzge9o</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>beginner gel x :)</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzge9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1dzg7h4</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Had my nails professionally done today for the first time in 5 years… before and after!</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzg7h4</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1dzg6os</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>New to Gel-X</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyv0qxaepkbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1dzg5vk</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>my natural long nails :3</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzg5vk</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1dzg0fj</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Tried out some desert nails. Still trying to get better at photos 🫣</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzg0fj</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1dzfb4k</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Glazed nails</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzfb4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1dzagrg</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Gel manicure damage</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dzagrg/gel_manicure_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1dzesoh</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Seashell nails</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzesoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1dzeewk</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Glitter ombre</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzeewk</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1dzbhde</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Getting redone today and cut shorter. Should I get a short acrylic put over this halfway detached nail? (My natural nails)</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypqhqvrqqjbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1dzdn9s</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Inside Out 2 Nail Art</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzdn9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1dzdkdo</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>First time I made them myself</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yc73tnjw5kbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1dzdh7g</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time rose quartz and gel x </t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzdh7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1dzd2fx</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Simple but cute</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzd2fx</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1dzctwk</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Apres/DND</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3z1hzdlg0kbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1dzcr9j</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Basic Nail Care?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dzcr9j/basic_nail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1dzcr6h</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>I am obsessed with this new design</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzcr6h</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1dzcbie</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So proud of my Nails, in honor to my motorbike. They are fluorescent </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzcbie</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1dzc8qb</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Shrimp nails</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzc8qb</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1dzc6nc</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Some of my sets from the past few months</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzc6nc</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1dzc114</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>First timer</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzc114</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1dzbzjm</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>First time doing gel x nails on myself, any tips?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfzn5tmcujbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1dzbume</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>For all my haters that didn’t believe the polish was why my nails were lumpy</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzbume</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1dzbqzi</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Powerpuff Girls!</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wsugg1psjbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1dzbmqh</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>I love doing my mums nails</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzbmqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1dzbm35</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do i need primer and dehydrator to do press ons ? </t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dzbm35/do_i_need_primer_and_dehydrator_to_do_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1dzazxa</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just got my nails done for the first time! </t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/htkdpb61njbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1dzagur</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you like simple desings? Or bold? </t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtavt987jjbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1dzagi1</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>How can I remove my acrylics without acetone?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzagi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1dzafnw</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>She always let me freestyle</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mp1x1hyijbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1dzac9t</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>ive been wearing this for ever</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzac9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1dza9fs</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>How did i do???</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ktugwxohjbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1dza586</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>What would y’all pay for these.</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ta3ideugjbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1dz9npa</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommendations for art gel? </t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dz9npa/recommendations_for_art_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1dz9mka</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Ombré sparkles is always my go to. I can go a long time between fills without it being super noticeable lol</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz9mka</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1dz9kz2</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>My sister in law did a thing.</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz9kz2</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1dz95u7</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>french tip with a twist</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2rsj72l9jbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1dz8s09</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>New to Gels : Pride Practice</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz8s09</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1dz8b95</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>What colour would compliment my skin best?</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29zmkq5e3jbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1dz6yy3</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Eczema around your eyes can be a sign of a gel polish allergy</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dz6yy3/eczema_around_your_eyes_can_be_a_sign_of_a_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1dyrkmh</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Press-on nails or salon nails?</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyrkmh/presson_nails_or_salon_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1dyt1mw</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Best glue for press ons?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyt1mw/best_glue_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1dyvyv3</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>how do y’all get good nail pics?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dyvyv3/how_do_yall_get_good_nail_pics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1dz82mo</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>3 1/2 month nail growth</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gce4orn1jbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1dz80eo</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t xml:space="preserve">help please! (nail glue) </t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dz80eo/help_please_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1dz7c7j</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Just finished painting my first ever set of French nails!!! (Regular polish)</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz7c7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1dz6rej</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Beach vibes. What do y'all think?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz6rej</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1dz6r62</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>My next set idea</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9uk46rq5sibd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1dz6lxl</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>growing my nails as a nail biter. any tips?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz6lxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1dz6chb</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Green and purple? Yes! 🌲☔️</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz6chb</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1dz5v7z</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>I love nail desingn for my week.</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz5v7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1dz5q03</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>What are a good nail option for someone who wants to remove them quickly when done?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dz5q03/what_are_a_good_nail_option_for_someone_who_wants/</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1dz5oti</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Are my nails too much?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz5oti</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1dz5glb</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Simple design... do you like it?</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjrvwlwuiibd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1dz59ac</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Is this how gel polish is supposed to look on natural nails?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0l7jt6gehibd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1dz56rt</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Summer coloured tips</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0esbl7xwgibd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1dz43un</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Are my nails too cutesy?</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz43un</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1dz3z4o</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>until it came out wordy! 😮‍💨🎀. I hope you like it🫶🏻</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz3z4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1dzowk0</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>How do I express to a nail salon that I’m picky about manicure quality?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dzowk0/how_do_i_express_to_a_nail_salon_that_im_picky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1dzo8mu</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me find this shade please </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pu83e7w3rmbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1dznx3g</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Missed Out :( </t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dznx3g/missed_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1dznirn</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Anyone else have a job that makes it impossible to grow your nails out?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2oesff2jmbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1dznb7o</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Shout out cosmic polish</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dznb7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1dzmnb6</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Any server girlies have work-proof topcoat suggestions? What's the longest lasting and strongest?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dzmnb6/any_server_girlies_have_workproof_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1dzl5pt</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Maelstrom </t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzl5pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1dzkocf</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>We're All Mad Here</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzkocf</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1dzk4s9</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Mixing it up</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q8namdkemlbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1dzjs0r</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>ILNP nail polish</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dzjs0r/ilnp_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1dzio2o</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Get Lobstered</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzio2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1dzij93</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>👾💜🍊🌺</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzij93</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1dzi5l5</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Anyone use Nail Hoot?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzi5l5</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1dzhpvr</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Not terrible for an ametuer, but how can I improve?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9auysicn1lbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1dzhga2</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>experimenting with isolated chrome</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8mxuy9hzkbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1dzh9so</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>New job new nails ✨</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzh9so</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1dzh256</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Bajo las Frondas</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jm27gobcwkbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1dzf8vv</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>What else should I pick up?</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dzf8vv/what_else_should_i_pick_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1dzeneh</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Gold and white for the summer</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzeneh</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1dze04e</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Daytripper alternative?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzubfy149kbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1dzdz1h</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>What do you do with a broken polish brush</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzdz1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1dzdtqe</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>LA Colors Super Bloom</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mllccv6u7kbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1dzbrdb</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Encasing Mooncat bottles in packing tape.</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dzbrdb/encasing_mooncat_bottles_in_packing_tape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1dzb0t5</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Fancy Gloss restock?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dzb0t5/fancy_gloss_restock/</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1dzb0hr</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Birthday nails from PPG collection!</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8uv6zc5njbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1dzajcq</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>ABCs of polish! S is for Scofflaw Varnish</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/370bafamjjbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1dzagt2</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Orange sherbet jelly sandwich 🍦</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzagt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1dza9ul</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your nail painting must haves? </t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dza9ul/what_are_your_nail_painting_must_haves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1dz9ssu</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wow… I was blown away by this! </t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mcqe7n49ejbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1dz86rl</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Facial exfoliant for cuticle?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dz86rl/facial_exfoliant_for_cuticle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1dz7otj</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Has anyone gotten a response from Mooncat?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dz7otj/has_anyone_gotten_a_response_from_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1dz7mcu</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>My current Summer mani</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz7mcu</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1dz6n88</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Show Me Your Brightest Pinks</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz6n88</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1dz6dhn</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are the 3 most used up polishes in your collection? </t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dz6dhn/what_are_the_3_most_used_up_polishes_in_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1dz5wrk</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Rare Candy Nails 🌈</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz5wrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1dz5vn4</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>When your mani matches your baby</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0tjgfxvlibd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1dz5foz</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Bluebird Lacquer - Meowza! 🧡🩷💛</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz5foz</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1dz4q3j</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>How to Achieve a White Sugary Glitter Effect?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dz4q3j/how_to_achieve_a_white_sugary_glitter_effect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1dz4pq1</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Quite possibly the best formula for a neon orange I could find, and it's only $4!</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5tkgsxidibd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1dz3wdz</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Chemical X is a party on my nails</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz3wdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1dz3cud</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Fancy Gloss Toppers</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dz3cud/fancy_gloss_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1dz39ax</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Recently started doing my own nails and this is one of my top favorites right now!</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/zIoaz3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1dz391u</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enchanted by this color; is it pink? </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53txm7pl2ibd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1dz37ci</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer's The Month of June</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldmzbdk82ibd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1dz28yb</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just discovered a crack in my mooncat bottle, how likely is it that it's gonna get worse? </t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dz28yb/just_discovered_a_crack_in_my_mooncat_bottle_how/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1dz1d0z</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Advice on removing polish?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dz1d0z/advice_on_removing_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1dz01rd</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Polished for Days - Baja Blasted</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz01rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1dyzzq2</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Glazed donut advice? Pinky has a more sheer and nude base color. Is it better/worse than the others? Looking to improve and would love tips!</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dyzzq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1dyz3rr</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>ILNP vs HT linear holos?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dyz3rr/ilnp_vs_ht_linear_holos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1dzlov8</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Finished painting my bobs burgers nails set 🥰</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihc0he8s0mbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1dzlabh</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Summer Vibes</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/og64wuvzwlbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1dzl5mz</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Beginner GelX</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzl5mz</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1dzjpp8</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>A detailed video on making nail art gel</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5bg5tm0nilbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1dzizy9</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Hello beautiful people, how did they turn out, I just started?</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amta3jvfclbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1dzhqzf</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>glitter and more glitter, I love it</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oo2oyuyq1lbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1dzg5ol</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Nail Art on Broken Nails</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dzg5ol/nail_art_on_broken_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1dzexlw</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Nasty press on nails</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ey3uxogzfkbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1dzdrlk</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Koi 💅</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6h0xgtte7kbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1dzdfa8</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Christmas nails(December 2023)</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nh65t4hv4kbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1dzavry</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(from fall) I hand painted my first character </t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptd7j4z5mjbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1dz930d</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Cherry Nails!</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz930d</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1dz6pal</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>My first 3D shaded character 🥹 Maybe doesn’t look QUITE like Moana, but you can tell it’s a person at least 🤣</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz6pal</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1dz5gdm</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>It took me 3 hours for this...does it look good?</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7lo76wriibd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1dz56q0</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Summer🏝️☀️</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz56q0</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1dz4xj3</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Nail art, made in 🇦🇷</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhtc3qf3fibd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1dz4fwd</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Nails kawaii  by street nail art 🇦🇷</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7igh88lbibd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1dz3tfe</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts?? Did this set for myself 🥰 </t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz3tfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1dz3tac</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>new month new nails</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7in053y6ibd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1dz3d6i</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Fancy Gloss Toppers</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dz3d6i/fancy_gloss_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1dz2glr</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Nail stamping: your favorite templates?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1dz2glr/nail_stamping_your_favorite_templates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1dz21nh</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>My beginner attempt 🥰</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ubfpbgq0thbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1dz08ob</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Strawberry season 🍓</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dz08ob</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jul 11 08:09:15 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_14.xlsx
+++ b/data/2024_07_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C652"/>
+  <dimension ref="A1:C830"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11517,6 +11517,3032 @@
         </is>
       </c>
     </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1e0jizv</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>What colour to paint my nails</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v77owdmhjubd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1e0h13y</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail appointment </t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e0h13y/nail_appointment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1e0j5ta</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> manicure UV light </t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e0j5ta/manicure_uv_light/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1e0j65v</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Hi all, one of my nails unfortunately broke, i only got them done about a week ago, what can i do? Can my nail tech fix just the one nail? Thanks</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svpbs0hweubd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1e0j21u</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My summer nails 💅 </t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0j21u</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1e0ifq2</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>My newest creation 💙💜🌌</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0ifq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1e0ieie</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Garden in hand 🌷</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aynbc0zm5ubd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1e0hxua</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Correct application DesignX Pro </t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0hxua</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1e0hn6n</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>My work of 2024 so far 💗</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0hn6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1e0hgko</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>so excited to find a page i can show off my nails</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0hgko</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1e0hfqa</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Trying to do the “clean girl” nail trend but don’t know if these look too plain?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzex6gp5utbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1e0hc2c</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>My natural length!</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7us8k5zstbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1e0h5nd</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>5 month growth progress 💕</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0h5nd</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1e0gghq</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>I’ve been doing my own nails at home for two months now 😭 do you think I’m ready to try and do some designs?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3ey3wyejtbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1e0g2vf</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Thoughts on my new French mint blue nails?</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0g2vf</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1e0g0ed</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Im calling this Holographic Cottoncandy</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/375htx2qetbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1e0fcgs</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Told my nail tech I wanted sugar and flowers and she took it from there 🥰 by @ xoyanie</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3crx5jc58tbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1e0f79l</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flowers for summer 🌸 </t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/895pfwes6tbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1e0f5tp</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Tried something new…</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0f5tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1e0f480</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>My wife’s set for a upcoming wedding. I think it’s one of her best yet!</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfiqx9sz5tbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1e0f24p</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Too much?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0f24p</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1e0f0y4</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Question about dip powder</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e0f0y4/question_about_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1e0ewgs</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Update to my nail shape I got a different style! I love it</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0ewgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1e0ej15</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Summer nails, anyone?</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0ej15</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1e0dmst</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Square French forever has my heart ❤️</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpaiabm8ssbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1e0dbbn</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Can I paint over gel nails with gel polish?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e0dbbn/can_i_paint_over_gel_nails_with_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1e0d3sr</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Nail done 😍</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0d3sr</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1e0czc3</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>strawberry nails</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emn5agjgmsbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1e0cjpp</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>What do you do with the underside of your press ons?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0cjpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1e0ci6y</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Decided to bling out for July </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhskni48isbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1e0bxux</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>cuticles are in pain :/</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e0bxux/cuticles_are_in_pain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1e0c95e</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail surface cleaner! Cleanser? </t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e0c95e/nail_surface_cleaner_cleanser/</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1e0c6i0</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time in forever! Something simple 🩷</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ji17vyefsbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1e0bt37</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Unintentionally matching my 🪥</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcfppe96csbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1e0boyv</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Small accident, removed press on and did gel manicure </t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0boyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1e0bi0v</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Synthwave, eat your heart out</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ny6rpauk9sbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1e0b031</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>What do you think of my cat eye nails? It's only my 3rd time ever getting my nails done and this is the first time I've tried this shape. I used to think square was my shape, but I actually love this!</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0b031</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1e0azv8</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t xml:space="preserve">and this is why gelx is superior </t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0azv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1e0az6q</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Totally out of my comfort zone! I feel like 🌸 Enid and I’m a 🕷️ Wednesday!</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ht9tevs85sbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1e0axw9</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Obsessed with my new nails!</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0xi463y4sbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1e0ao63</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Blue 🌊</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0ao63</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1e0alyg</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Bright pink for summer</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0alyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1e0ak7b</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>My nail lady gave me unexpected butterflies 🦋</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/daw154gu1sbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1e09027</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>I love my nail wizard so much!</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsmz26foprbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1e08e99</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Looking for a specific charm</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4asslddblrbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1e07uro</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1h55pibhrbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1e0agzh</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Proud of my DIY natural nails!</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2x7skx41sbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1e0agh6</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Tomorrowland Ready 😈</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5m3cexc01sbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1e0a83s</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>She kills it every time😭❤️</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lt67jn5zrbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1e09uz8</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Obsessed with this color 😻</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tx8e2v8wrbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1e09t4t</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>loving the crocodile vibes</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e09t4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1e09dsl</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone ever ordered from the DND website? How long does it take to come in? </t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e09dsl/has_anyone_ever_ordered_from_the_dnd_website_how/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1e093m8</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Any tips or hacks to grow my nails.</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxzwdpxeqrbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1e08lc3</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>We all scream for Ice Cream! 🍦(Done by me, on me!)</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e08lc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1e07yec</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Love how these turned out - subtle but glowy</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eoxn0do1irbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1e07gpn</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Almond chrome French</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmhx1maferbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1e06xqe</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Can you use press-on nails to avoid getting a gel/acryllic allergy?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e06xqe/can_you_use_presson_nails_to_avoid_getting_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1e06blj</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Are dip nail liquids safe?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e06blj/are_dip_nail_liquids_safe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1e04j06</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍒💅 One week old. How do you take care of your original nails? </t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e04j06</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1e071hn</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Learning to make short nails look cuter one day at a time😌</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e071hn</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1e070yp</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The checker was done free hand today by the technician and I am beyond impressed! </t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e070yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1e06uki</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>first set in a year</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5hshn6y9rbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1e069sd</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>My take on Bee nails</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/112e3uxl5rbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1e06mqg</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Gel Nails vs Acrylic.</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e06mqg/gel_nails_vs_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1e060eq</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Natural nails with acrylic overlay! 😊</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ibb0jxs3rbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1e05q8c</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>New set opinions 👀</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e05q8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1e056l1</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This mooncat primer is pretty enough to be a polish on its own </t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfpfeimuxqbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1e04qh3</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>i buy this press on, , can you notice that they are "fake"?</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lt8hg7xhuqbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1e04n8s</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Summer Nails match my garden 🥰</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itbq7ueutqbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1e04n20</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Fun summer nails</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54f888bttqbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1dzzz5p</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Question about UV gel and regular polish</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dzzz5p/question_about_uv_gel_and_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1dzznra</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Isn't this spring inspired design beautiful? I love it!</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycudjatxtpbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1dzu648</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Did my own nails (with polygel) for the very first time!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/72mw4sexmobd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1dzmmx8</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Is this a good Job? Would you have said something to the technician?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzmmx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1dznywk</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Made my first press-on set</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dznywk</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1dzqdfk</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Had a go with my stamping plates. Only the second time. I used a purple, gold and blue polishes to get this effect.</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzqdfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1e00blv</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>How long is long enough to wait before I get these  removed (MMA may have been used)?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e00blv</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1e00jek</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>The Polish (Japanese jelly brand)--shipping to US?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e00jek/the_polish_japanese_jelly_brandshipping_to_us/</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1e00rq2</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>french manicure on clubbed thumbs</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e00rq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1e03203</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>OK, my last nail repair inquiry…</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e03203/ok_my_last_nail_repair_inquiry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1e03s5j</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>What style/length would suit me best / should I get? (pic #'s 1-3 are styles I've done in the past, 4a-e and 5a-e are some other styles I've considered... but not sure if I could pull off)</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e03s5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1e040xu</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Did these last night!</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e040xu</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1dzvv8d</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Nail tech cut me several places around my fingers - is this common?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzvv8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1e03p4u</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Can't have long nails anymore... a blast from the past! (Nails on me, not done by me)</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e03p4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1e03m2s</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>First attempt at nail extensions</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e03m2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1e03km4</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Shape decisions????</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e03km4</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1e036ap</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Gane time decision</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e036ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1e02rp7</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Short extension retention + rough edges near cuticle when nail grows out</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e02rp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1e01ofo</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Thoughts on thick French?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7t4z9kg8qbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1e01izg</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Need help color matching these press-ons</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e01izg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1e01ilr</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Acrylic Soak Off</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e01ilr</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1e01bfl</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>First time french tips</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ruo5ad7t5qbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1e01a6c</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>DIY gel-x</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hq8r16bj5qbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1e0130w</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Does anybody know where I can find a similar product? All the blank mail decals I can find are for printers. I want to paint on them. She sells out so fast 😩</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>http://www.marieevemongeau.ca/produit/cahier-stickers-autocollants-personnalises/</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1e00rf2</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>People who do press ons: what do you do with all the extra nail tips that don’t fit your nails?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e00rf2/people_who_do_press_ons_what_do_you_do_with_all/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1e00gaj</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Neon set</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e00gaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1e007ur</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Coffee tips..</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e007ur</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1e005ik</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Obsessed with this peachy color. Wedding guest ready!</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e005ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1e001iu</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>which drill for gel nail removal</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e001iu/which_drill_for_gel_nail_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1dzzs1a</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Builder gel advice</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dzzs1a/builder_gel_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1e0je4m</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Nail polish recommendations for Indian skin tone / wheatish skin tone</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5699pzarhubd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1e0hs3d</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Mooncat Ghosts of Hecate Combo 🍩💙👻</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s740yhf5ytbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1e0gvdx</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>5 Month Growth Progress!</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0gvdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1e0fdij</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t xml:space="preserve">it’s giving chevron era watermelon </t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77lozpmf8tbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1e0f88z</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>So bright my camera couldnt capture it</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6uqtj7i17tbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1e0cx7s</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>D.H Purple Glitter</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/ItRgfeD</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1e0cix7</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Looking for your chunkiest, flakiest, shiftiest, glittery favorites!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkwoe76eisbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1e0ciwu</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Powerpuff Girls Stamping</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0ciwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1e0chni</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Decided to bling out for July</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyb5gqc3isbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1e0cgsv</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>I have a mild gel allergy and i dont want to make it worse. Are press-ons safe?</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e0cgsv/i_have_a_mild_gel_allergy_and_i_dont_want_to_make/</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1e0b03p</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deep Blue Gel Manicure </t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0b03p</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1e0azov</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Mooncat The Diabolical Mojo Jojo!!</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gw125cmd5sbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1e0ajrc</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Clown Nails</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0ajrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1e09wj4</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Clearly this has not been my week 🙃 (swipe to see closeup!)</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e09wj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1e09tep</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>this is your sign to buy flower child 🌸</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e09tep</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1e09iby</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Show me your perfect red!</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujty0f9itrbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1e092pd</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>I caved and ordered some Glisten &amp; Glow!</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydyxe7b8qrbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1e08xqm</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's a floral kind of day </t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e08xqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1e08pu7</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Toddler nail polish?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asqeqojlnrbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1e08o33</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Help, splitting nail</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8jew6g9nrbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1e08466</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Color Therapy Mani!</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e08466</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1e07x0u</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>How do I make the gradient blend more smoothly?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e07x0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1e071s3</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Had gel extensions yesterday after not having a manicure for 5 years!</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hxmblrebrbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1e071dv</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Ice Cream nails</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e071dv</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1e063oi</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Thermal polish is so fun!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e063oi</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1e05pjm</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am obsessed. </t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e05pjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1e05nx4</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lamp for cheap Amazon polish (application on press-ons, not natural nail) </t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3u07laa1rbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1e04e1o</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>OPI-Can't Find My Czechbook</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e04e1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1e045w5</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Previous nail biter!</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvgxgxd9qqbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1e044gi</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Finally got my hands on Indomitable and I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e044gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1e03ia7</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Summer is for building sand castles 🏖️🪣</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e03ia7</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1e03bje</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Maelstrom ✨</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e03bje</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1e02m4j</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Polish Storage </t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e02m4j/nail_polish_storage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1e02fqb</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s giving I trapped dirt in my topcoat (but I like it) </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e02fqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1e01qtm</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Manicure day 10</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7972od1y8qbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1e00zff</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shamrock with a flakie topper! </t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e00zff</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1e00xn2</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Holo powders are GORGEOUS. 10/10 would recommend</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e00xn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1e00mhn</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Wishlist App???</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e00mhn/wishlist_app/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1e00j7j</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t xml:space="preserve">recs for polishes w/ micro holographic flakes + strong shimmer </t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e00j7j/recs_for_polishes_w_micro_holographic_flakes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1dzzug7</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Looking for a dupe--rusty orange with a jelly vibe?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zuj86ss8vpbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1dzzadx</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>I love this topper so much</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzzadx</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1dzz5us</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Finally tried Orly 🤤🔥🧞‍♀️</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzz5us</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1dzy0di</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>💦🌊Water🌊💦</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzy0di</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1dzxxpa</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Saved by the Bell vibes</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzxxpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1dzow9e</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Gold’ish olive skin - specific polish suggestions?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dzow9e/goldish_olive_skin_specific_polish_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1dzxvzr</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Today I learned that solar polish doesn’t mix well with top coat</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzxvzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1dzxh1r</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>European base + top coat recommendations (+nail polish)?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dzxh1r/european_base_top_coat_recommendations_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1dzxgkx</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Decanting polish - recommendations for empty bottles with wide brushes?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dzxgkx/decanting_polish_recommendations_for_empty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1dzxckn</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Ver much digging The Diabotical Mojo Jojo</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzxckn</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1dzws1t</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>I Want My MTV (Solar)</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/twnsq4ds8pbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1dzw3xp</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Psionic- velvetized</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hwtannmi3pbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1dzvsq6</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Those with the horseshoe magnet please advise 🥺</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dzvsq6/those_with_the_horseshoe_magnet_please_advise/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1dzvptc</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>When your best friend is defending her neuroscience thesis, you do nail art to support her!</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzvptc</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1dzvhui</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Friends and I had our nails done</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q47l0wziyobd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1dzu76i</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>RV there yet</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qb58pn87nobd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1dztvlq</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>top coat dulling/looking matte on nail tips ??</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmpmgsi9kobd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1dztgpj</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Soooo Pretty</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dztgpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1dzt6tu</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Pink Jelly Nails I Did a While Back~</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwtqdy8cdobd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1dzrzi1</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>HHC Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dzrzi1/hhc_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1e0hzni</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>It's really super beautiful!</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0hzni</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1e0gpz7</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>I did these tonight in class! What do y’all think 🥰</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0gpz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1e0gkx2</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Just starting out. What do you think?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03f2tt7oktbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1e0eg1k</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Purple purple purple</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59mrqizrzsbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1e0d7mk</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>A detailed video on making nail art gel</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zszbcc8bosbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1e0bj0e</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Synthwave, eat your heart out</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20q9ncxs9sbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1e0900e</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Did these myself(sorry about the snapchat filter but it’s the only photo I got) what can I do to make them “less basic”?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1bwhy0oprbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1e07rja</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need your honest opinions. Is it good? </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqhy5iwmgrbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1e07fnf</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>I need ocean nail recommendations. I really like this blue French tip but fell like it needs a twist.</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tu29bow7erbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1e06auj</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>🐆</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uv52qouu5rbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1e04hkx</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Hand painted Spirited Away nail art</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0y6u0dpsqbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1e03zjj</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>spring design 🌸by Ksnails</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8o7tc2gjoqbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1e038hr</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>In love whit these colors and this de design inspired in shinobu kocho ❤️‍🔥❤️</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imfw86mjjqbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1e02n8m</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Polish Storage </t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e02n8m/nail_polish_storage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1e00jrz</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Neon set</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e00jrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1dzyhez</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>First time double ombré french! So much fun 😊</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o50pm4eilpbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1dzujx5</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Celestial </t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dzujx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1dztx3k</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>I hope you like them, they match my motorbike</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1y4jxeunkobd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1dzsr77</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Catholic inspired set my friend made for my mom </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/walddmzw8obd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jul 12 08:10:13 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_14.xlsx
+++ b/data/2024_07_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C830"/>
+  <dimension ref="A1:C992"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14543,6 +14543,2760 @@
         </is>
       </c>
     </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1e1c60b</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gelx nails don’t respond well to e-file </t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1c60b/gelx_nails_dont_respond_well_to_efile/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1e1bqmx</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>🌸💅</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/quf8if5tj1cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1e1amgi</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>This is my first set of gel x nails ever!!</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1amgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1e1aimv</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>GelX Popping off of Builder Gel</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1aimv/gelx_popping_off_of_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1e1aeyw</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>affordable gel polishes??</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1aeyw/affordable_gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1e1ae3j</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Struggling to go back to short nails…</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0aug7r5941cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1e19k0o</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Had my nails done professionally for the first time</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e19k0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1e19h9o</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Been learning how to do gel x nails! I wanna learn how to use builder gel 😅</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e19h9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1e19del</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried a new shape and was mesmerised by the glazed pink in the sun this morning while picking my 🍋 </t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e19del</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1e19bm7</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Do you think it's suitable for my upcoming beach trip?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okv53usis0cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1e0ydbu</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>How do I fix/prevent this?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omisb9ji5ybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1e17mm3</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bt21 gel nails </t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e17mm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1e0y86q</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Got my gel nails removed and a basic manicure (no color polish) and this is how my nails look. Is this normal/acceptable?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0y86q</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1e0z68x</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Cryl or gel!?!?!</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e0z68x/cryl_or_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1e1213b</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These are awful, right? They’re $120 and the first set of acrylics I’ve gotten. </t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1213b</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1e12oed</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>remove acrylics after a day?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e12oed/remove_acrylics_after_a_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1e1355j</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t xml:space="preserve">✨ OPI in Scorpio Seduction ✨ </t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/moyz2ohz6zbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1e147n5</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Do you like?</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpzjvaxdgzbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1e1684t</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>kds nail glue is not doing it for me 😭😭 any glue recommendations?</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1684t/kds_nail_glue_is_not_doing_it_for_me_any_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1e16sz5</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>If you zoom in, Hello Kitty has a surprise.</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e16sz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1e18vbh</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I started making press-on nails! So excited to get better. </t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e18vbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1e186mg</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>my favs so far</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xyx9eyzah0cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1e17fyc</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Black 🌚💎🧿</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e17fyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1e17edo</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Essie Ballet Slippers</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfb70r2n90cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1e16vqa</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Is peel off liquid latex okay for gel nails/UV light?</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e16vqa/is_peel_off_liquid_latex_okay_for_gel_nailsuv/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1e16vkq</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Does this round/oval shape suit my hand? I’ve only ever gotten square or coffin.</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qes952hs40cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1e16klt</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Tribute to my dad who passed away</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e16klt</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1e16ndc</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Short nail appreciation post</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e16ndc</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1e16mpb</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Hello Kitty nails 💕✨</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nk4ls4i20cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1e16mgm</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>3rd gel set at home</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e16mgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1e16dyu</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>i got my nails done for the first time ever for my sister's wedding and ~*~*~ 🥰💅💞</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e16dyu</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1e16agh</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Groovy Bridal Shower Nails 🥰</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e16agh</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1e165uw</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Gel Nails</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e165uw/gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1e15zse</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>I love red manicure 🥰 Classic</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2t8wq2spwzbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1e15yie</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A nice holographic ombre for summer </t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/os0rw40ewzbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1e15yfm</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Don’t know names of nail treatment/ design types</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e15yfm/dont_know_names_of_nail_treatment_design_types/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1e15515</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Cat eye polish</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e15515</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1e14yif</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Love bubble baths and glazed donuts but this I can stare at for days</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e14yif</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1e14xvj</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Ouchhhhh - rip to this set</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ijj284lzmzbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1e14xn8</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art in a long time! (Geli Potion brand gelx)</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e14xn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1e14lvy</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Probably my fav nails ever🤩</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e14lvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1e14jhm</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech was saying ‘I’m not used to your nails looking so simple!’ And kept grabbing my hand to look. I always do  nail art 🥹 peach nude jelly nails </t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nv21hmadjzbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1e14gne</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Custom press ons by LowKeyNailed it</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e14gne</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1e14dfg</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Why does underneath my nails have dead skin that was attached to my skin, coming up and flaking off ??</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lizapnrthzbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1e14blo</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Help 😩</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e14blo/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1e14b6n</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Hello Kitty Nails with Dip Powder for my birthday</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xf1odzm9hzbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1e14b6a</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did some cute nails today. </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpp8fyd9hzbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1e143w7</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>My nail tech SLAYS 💅</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26z79ukgfzbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1e1422y</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Did some quick summer nails for myself 🌞</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcbxogszezbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1e14212</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just did my nails today </t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wv5sn37zezbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1e13pec</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>BUTTER NAILS</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e13pec</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1e13o3x</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>How can I get better at shaping my nails?</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e13o3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1e137il</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>My New Obsession: Rainbow Cateye</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1grgw35j7zbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1e12jsj</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Some of the designs of my “nail history”</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e12jsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1e12ipc</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>263829 hours later</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e12ipc</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1e12dw1</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Did my own nails for the Blink-182 concert tonight 🤩</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e12dw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1e12bkf</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Nails I did for sister in law</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e12bkf</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1e128nj</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Bit of color for the summer</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0je1s5izybd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1e125hq</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💅 </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e125hq</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1e11usz</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>It’s giving Beauty &amp; The Beast</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e11usz</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1e11dbv</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why doesn’t my BIAB stay on my thumbs? </t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e11dbv/why_doesnt_my_biab_stay_on_my_thumbs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1e1194u</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Emerald Green</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjes5mpirybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1e116pk</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>are these bad or am i too picky?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2quov0lzqybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1e114g1</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Confused with aftercare when getting nail extensions </t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e114g1/confused_with_aftercare_when_getting_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1e11253</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm trying out these new nails from my bestie, are they too long </t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqvgjmmzpybd1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1e10crh</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>🍋🍋🍋</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t19573pikybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1e104sb</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Matching my nails with my jumpsuit- ready for PBE 🌹!</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02sxppfuiybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1e10092</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Acrylic System recommendations</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e10092/acrylic_system_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1e0zket</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>creases in gel nails?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0zket</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1e0zf75</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Nails grow up from nail bed?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0zf75</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1e0zd7f</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>in lovveeee ⭐️🙂</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ilit8dvcybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1e0ydzz</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>do dip nails cause allergies?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e0ydzz/do_dip_nails_cause_allergies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1e0xd3s</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Jhene AikoConcert Inspired</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmhjtkk2yxbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1e0w57b</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>does nail aid REALLY work?</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0w57b</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1e0vvsa</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Nail tech cut me several places around my fingers - is this common?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0vvsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1e0ytsx</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Been learning how to do my own gel manicures and my nails are getting so long! </t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oucrxovx8ybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1e0yl2o</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Love these😍😍</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4djo68o47ybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1e0yddi</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fs3q1mti5ybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1e0ybdg</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>What nail shape would look best for my hands? These are 2 I have tried.</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0ybdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1e0xxo2</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Did my own nails</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9eeys9b2ybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1e0xnts</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>What color nails with this suit for a wedding?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ten8sghb0ybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1e0xkj7</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Fresh chrome set</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2h3bqj5mzxbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1e0xjdb</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Recently my favorite polish :)</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0xjdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1e0xi0u</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Purple Sparkles and Flowers</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0xi0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1e0xfpk</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Going minimalistic :)</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwza1cnlyxbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1e0x8g5</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Natural nails</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcsn9mk2xxbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1e0x1t4</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Halo 💙</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/um29oiznvxbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1e0wo2h</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0wo2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1e0w4am</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Baby blue chrome</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4n6zjyokoxbd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1e0vj9a</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Does this look weird ?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0vj9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1e0vi2a</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>First time doing press ons</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/byqqk3hxjxbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1e0vg3l</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>I told them my idea and they DELIVERED 🦋</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0vg3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1e0vexk</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Hurricane Beryl vs Extendos</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b39m640ajxbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1e0v2nu</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Basic, but I love how simple it is. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0v2nu</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1e0uuwx</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any gel lamp recs? </t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e0uuwx/any_gel_lamp_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1e0uitv</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Is it possible to fix this?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e0uitv/is_it_possible_to_fix_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1e0fs5a</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>ways to cover a torn-off nail?</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e0fs5a/ways_to_cover_a_tornoff_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1e0u4hi</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dragonfruit inspired by my tech J in Chicago </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23gtgfsn9xbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1e0ucm3</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This just.. Yes! </t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/586js66dbxbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1e0smw8</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2w8vd3hywbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1e18ley</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>R/Odd life confessions</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e18ley/rodd_life_confessions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1e18p31</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>I just unsubbed from r/calmhands</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e18p31</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1e18cjo</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Big Bird!</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txaxujpsi0cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1e17d5z</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Baptism by Fire 💚❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e17d5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1e16wnz</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Bees Knees’ Arcana velvet. Hnnnggghhh.</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nyw7n62z40cd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1e16jso</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>3rd set of gel at home</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e16jso</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1e15tqw</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>I didn’t think I would like this as much as I do!</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e15tqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1e14wfu</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fun day pastels for the summer </t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e14wfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1e14rar</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Mercury’s Tears</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvai23ddlzbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1e13qx6</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Indies Down Under</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e13qx6/indies_down_under/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1e13ggq</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>How to make chrome nails last?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e13ggq</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1e130r5</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Little Mermaid Top Coat Experiment (with bonus K&amp;Co I Want My MTV)</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e130r5</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1e12skz</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Great Lakes Lacquer Haul</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pba3i9j04zbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1e12dtc</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>What’s the most dangerous thing you do with your nails on a daily basis?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e12dtc/whats_the_most_dangerous_thing_you_do_with_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1e12cmt</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Helllppp</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e12cmt</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1e12490</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Emily de molly</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e12490</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1e11uak</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>top coat shrinkage</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqghsxc5wybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1e10u6c</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Powder Question…</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e10u6c/powder_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1e10g58</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Do y’all also collect top and base coat?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dd9fwg8lybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1e102qv</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Matching my nails with my jumpsuit- ready for PBE ❤️</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8p1u0eeiybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1e1012u</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>In love with this magnetic topper</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ll65ow51iybd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1e0zt2m</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>BKL “The Twin Alders”</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjinpp2cgybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1e0z3rk</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Essie wicked 🖤</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6f2ol0wyaybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1e0yrvs</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>mooncat mani, no bloodshed! (shade: Merkitten 🧜🏽‍♀️🐱)</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02ge9xxj8ybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1e0y719</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Grungy nails for miserable weather!</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0y719</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1e0xl1w</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>empty bottle recs</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e0xl1w/empty_bottle_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1e0xk3m</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Purple Sparkle and Flower Nails</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0xk3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1e0xf1h</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swatched my birthday haul </t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bc5zjqvgyxbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1e0xary</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>New favorite polish! L.A. Colors’ Ravishing Gown</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0xary</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1e0u4n6</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Non-gel topcoats from chrome powders </t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0u4n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1e0t4hx</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>How would something like this be achieved?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38wwu1932xbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1e0sdga</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Bottles with same neck as Mooncat?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e0sdga/bottles_with_same_neck_as_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1e0qm5t</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Black and White Flowers</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zkwr5m5jwbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1e0pp4u</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Shiny pink!</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pdsmvd4zbwbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1e0pjb1</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Dragon Scales is a trip!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifsrelxeawbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1e0n8sx</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Back at it!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e0n8sx/back_at_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1e0l758</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Phoenix Indie For Rocket is SO good 😭💖</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0l758</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1e0kesm</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>I'm terrible at crosswords...</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4cunr7suubd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1e1apbb</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A detailed video on making nail art gel </t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hlvkglmc71cd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1e19ud6</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Nail stamping issues</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e19ud6/nail_stamping_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1e18zv6</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Started making press-one, can’t wait to keep improving! </t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e18zv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1e18zdf</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Looney tune nailss</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e18zdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1e17q25</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>I wanted to highlight the design with the crystals, do you think I achieved it?</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dw55z6qpc0cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1e16kzo</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Short nail appreciation post</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e16kzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1e141cs</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Did some quick summer nails for myself 🌞</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mcod57tezbd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1e13ibp</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Milk blue nails, chipped. Advice on how to fix?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e13ibp</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1e12vh9</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>I want to recreate this design, what do you think?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qiyh3go4zbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1e12v1p</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Went a bit crazy on the colors...is it good?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09p2l5fk4zbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1e1251x</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Strawberries</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynlfreqmyybd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1e11acf</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>First time attempting a 3d design (I’m aware she’s very wonky)</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e11acf</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1e0y6j2</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried nail art for the first time. Definitely harder to do than I thought it would be </t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0y6j2</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1e0wtl8</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Practice work - help me</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0wtl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1e0wskk</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>This weeks set 🎰</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32b4ubfptxbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1e0w7d3</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Honey bee nails</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0w7d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1e0w4bx</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I really love butterflies 🦋 </t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qe7irpmloxbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1e0u4aq</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Up🩷🩷</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x37zse9m9xbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1e0u17c</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Violet flowers💐🪻</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0u17c</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1e0tyco</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anime inspo </t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0tyco</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1e0twwa</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>gravity falls instó</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0twwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1e0rvvs</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Demon Slayer </t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0rvvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1e0ppv5</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wholesome fish skeleton nails </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ksc63tm4cwbd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1e0laoh</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Longlegs 🔪</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e0laoh</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jul 13 08:07:52 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_14.xlsx
+++ b/data/2024_07_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C992"/>
+  <dimension ref="A1:C1168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17297,6 +17297,2998 @@
         </is>
       </c>
     </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1e250j3</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Please give me your thoughts about my nails -DIY</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e250j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1e248rc</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to ask for service </t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09fr6dfjj8cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1e23zkb</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>My summer nails, that I wore in June</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e23zkb</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1e23d4t</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>What color should i paint them</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irvga4dl98cd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1e23r5y</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>First nail art set!</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/435e3wmvd8cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1e232y5</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Hard gel and drill suggestions</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e232y5/hard_gel_and_drill_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1e22kbv</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Birthday nails 🌸🎈</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e22kbv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1e22hxi</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Vertical cat-eye featuring my emotional support iced americano</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e22hxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1e22234</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>are pressons a desire?</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e22234</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1e20l10</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Thinking about getting a manicure for the first time and need guidance</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e20l10/thinking_about_getting_a_manicure_for_the_first/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1e205ee</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Acrylic overlay SUFFERING</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e205ee/acrylic_overlay_suffering/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1e1zlvg</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Sharing for inspiration</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/skw1czj677cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1e1xt1d</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Help... it is so bad</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yketg7zoq6cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1e2292b</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>I love how simple they are but I think they were too long.</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/op9yn1z4x7cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1e226h8</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t xml:space="preserve">help: retention sucks for 1 specific finger </t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e226h8/help_retention_sucks_for_1_specific_finger/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1e2151a</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Sparkles and Flowers Nails!</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2151a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1e210hn</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>How to fix?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a776cypkk7cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1e20ulq</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seche Vite: whoever recommended it to me, I Love You </t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e20ulq/seche_vite_whoever_recommended_it_to_me_i_love_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1e20k9h</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Heart and swords ❤️‍🔥⚔️🖤🗡️🔥</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e20k9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1e20hms</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Summer sunflowers ☀️</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kr7mhkrgf7cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1e1zpw5</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>help</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1zpw5/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1e1zlb0</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Summer vibes</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1zlb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1e1z94d</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>How much is too much to use a uv lamp (on your own nails)? How often do you use a uv lamp on your nails?</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1z94d/how_much_is_too_much_to_use_a_uv_lamp_on_your_own/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1e1yy3t</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Ocean tie dye</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9s12lw217cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1e1ywcx</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Wedding time!!</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1ywcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1e1ye3l</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>I just got them done and I love them!! 💖✨</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1ye3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1e1yd0z</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Tried a new color, I feel like it’s too bright 😭</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1yd0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1e1y29k</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>My first time getting my nails done, in love! 😍</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1y29k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1e1wyzp</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Nail polish remover</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1wyzp/nail_polish_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1e1wxv3</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Intermediate E-File Help</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1wxv3/intermediate_efile_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1e1wo1a</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>2nd DIY set</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1wo1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1e1wigi</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b36lfpadf6cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1e1vgc8</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Went to a New Nail Tech and Wondering if I Should Be Concerned...</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1vgc8/went_to_a_new_nail_tech_and_wondering_if_i_should/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1e1ugv0</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Tried to do a velvet-to-jelly ombre, but it looks like I have a scab under my nail at some angles 😭</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rised2ksy5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1e1w4ia</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Taking a break from plain nails</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obyy6lt2c6cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1e1vhxz</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Finally done 😌</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1vhxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1e1uhe3</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Nail day is always a happy day!</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03xtnmkwy5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1e1ufy0</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>My new nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtumvgcly5cd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1e1ufms</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>New Dip Powder Design</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4pfca1riy5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1e1uexa</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>did these myself what do yall think?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1uexa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1e1u1qg</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Pink cat eyes</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3yvg4xlv5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1e1tuew</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>I love this color!</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gd2fjjp3u5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1e1trt4</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>My husband said my nails look like poptarts 😭</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1trt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1e1trhi</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Juicy</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjp3xqkgt5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1e1soq2</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>I wanna stop doing nails</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1soq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1e1t4t2</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Summer Aura turquoise nails + chrome</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1t4t2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1e1tjmr</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>House MD inspired mani</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1tjmr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1e1tm9m</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>My last hurrah for a little while!</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8iar7vcs5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1e1ss20</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>ILNP-Poison x My Private Rainbow X</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1ss20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1e1sr00</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>pink 💕 pony 💕 nails ! First time doing chrome power on myself!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03f939vtl5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1e1s8fv</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Bumps in chrome</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mtax2dyh5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1e1s89s</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Went to a new nail tech 🥰</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbyuywixh5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1e1s1mo</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Got my first pair of gel x!</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1s1mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1e1rnon</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Is the GAP that bad omw to somewhere nice - I’m getting them redone Sunday</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c592a8od5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1e1rcb9</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Y2K inspired pink leopard nails</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvwpqqi8b5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1e1qzp0</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why does my nail polish always peel off the next day? </t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1qzp0/why_does_my_nail_polish_always_peel_off_the_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1e1rcj4</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Thank you guys🫶</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrwwoq3ab5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1e1rch2</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First to Second BIAB set (7 Weeks growth!) </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1rch2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1e1raxy</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Best Glue for Press-on</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1raxy/best_glue_for_presson/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1e1r5v4</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Went back to gel x</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1r5v4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1e1qp0u</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Magic color 💫⚡️🌟💚</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1qp0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1e1qdyy</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>How can i get rid of this weak line on my nail?</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16mspii245cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1e1pili</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Broke 2 nails 1 week after Dip Powder.  Help?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1pili/broke_2_nails_1_week_after_dip_powder_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1e1qaxs</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Not my OC but I love this channel: 영네일 YOUNG NAIL on Youtube - Nail ASMR</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://youtu.be/2jn-8doWLIM?si=3fTtD1uJXqdIc0th</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1e1pupf</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>DND Lamp</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1pupf/dnd_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1e1pmbu</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>paid $120 for these plus another $25 for a soak off, do u think it was worth it?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vmz1x3y9y4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1e1p10c</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do my nails just grow fast or is this normal? 13 days post manicure. </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtyd1dftt4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1e1ozx3</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Show me your bridal nails!!</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1ozx3/show_me_your_bridal_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1e1oy1l</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Watermelon Nails</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1oy1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1e1ovwg</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Builder gel saving my life…</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3j80f2aqs4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1e1osnd</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>I love my warm chocolate BIAB nails 🍫🍪</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1ej9q02s4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1e1oro7</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Essential nail polish collection</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1oro7/essential_nail_polish_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1e1oql1</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>I quit</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg20frbmr4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1e1og43</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t xml:space="preserve">watermelones🍉 </t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag29rujep4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1e1klv9</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Possible gel allergy?</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1klv9/possible_gel_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1e1jfis</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails are gone 😭French tips ? </t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1jfis/my_nails_are_gone_french_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1e1ncrs</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For the “do my nails on my own” girlies: How often do you switch up your colours? </t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1ncrs/for_the_do_my_nails_on_my_own_girlies_how_often/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1e1nc3v</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Keep or change shape? My nails vs Inspo from Pinterest @annarose_brennan</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1nc3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1e1jx66</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>New set ‘Punk’ part I</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1jx66</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1e1odhm</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Product Called Zen Builder Gel</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kux3l3zvo4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1e1o26r</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1o26r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1e1nqzl</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm soo happy with how this cats eye gel came out! </t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k9a4uobak4cd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1e1mumy</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vln61kgnd4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1e1mk8k</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>First time I had my nails really done ❤️</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgnhp06lb4cd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1e1fsvi</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1fsvi/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1e1grx5</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>For what occasion would you use these nails?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mo41py6533cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1e1hwtg</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Is it worth it to switch from sticky tabs to nail glue?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1hwtg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1e1jkft</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Low rider nails🤩</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1jkft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1e1ljr6</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>What can I do to spice these up?</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kydsti444cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1e1m8n1</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>slay or nay? 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh5byac694cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1e1m11q</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Energy drinks are growing my nails</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4s7hn3am74cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1e1lz2p</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech is the best </t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tx6sdoq874cd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1e1lsdc</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>DIY nail extensions/longer nails</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1lsdc/diy_nail_extensionslonger_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1e1lo40</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1lo40</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1e1lk69</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Are there any shapes I should try to make my hands look a little more feminine and flattering?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1lk69</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1e1lg2c</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Lifelong biter, stumpy fingers, toe thumb 😵‍💫😵‍💫 how can I improve?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1g71bdd34cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1e1krcz</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Indian summer🧋🧋</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txorpejey3cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1e1jkgt</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Dip Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e1jkgt/dip_wedding_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1e1jjba</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Absolutely obsessed with my new nail set!  What color should I go for next?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1jjba</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1e1i8rg</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Cottage Core For Dayzzz</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvqkvb4af3cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1e253qc</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>How do Russian Manicures grow back?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e253qc/how_do_russian_manicures_grow_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1e25387</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>mooncat mercurys tears</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e25387/mooncat_mercurys_tears/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1e23gjx</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Mermaid nails 🌊🐚✨</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kok71lcma8cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1e22tsf</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Transitioning from nail enthusiast to nail tech </t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e22tsf/transitioning_from_nail_enthusiast_to_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1e22bwu</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Talk me in or out of this guys and gals. I'm pretty positive the yellow shade is the only one I wouldn't use on the reg... Price in AUD </t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l33o72yzx7cd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1e21swc</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>What on earth happened to my fingertips??</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vutywrmbo7cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1e217il</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Flowers and Sparkle Nails!</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e217il</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1e20v30</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seche Vite: whoever recommended it to me, I Love You </t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e20v30/seche_vite_whoever_recommended_it_to_me_i_love_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1e209ux</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Zoya shimmers disappointing?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e209ux/zoya_shimmers_disappointing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1e1yt0l</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Nail polish never lasts! </t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e1yt0l/my_nail_polish_never_lasts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1e1xip8</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think I found my perfect nude jelly? </t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1xip8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1e1x2da</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Since when are drugstore polishes so expensive D:</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkl3b5kxj6cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1e1wzeb</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>This looks familiar..</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1wzeb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1e1wjbr</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Something angelic and sparkly</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1wjbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1e1we86</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Sun prism power, make up!</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://imgur.com/ZZv0pOd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1e1vfcw</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Lurid - Out on Your Street</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1vfcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1e1vew0</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Short, square &amp; pink 💘</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5w7urt9a66cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1e1v0zr</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Cheapest Clear Coats?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e1v0zr/cheapest_clear_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1e1v0lt</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Today I matched my Kindle</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1v0lt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1e1uv3g</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Sticking our Paws in the sand 🏖️</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1uv3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1e1uhux</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Pahlish - "Hoax"</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1uhux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1e1tpqo</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Playing around with a sparkly (mostly) ILNP skittle</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rys4y8fzs5cd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1e1thms</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>House MD inspired mani</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1thms</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1e1t6zm</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Summer Aura turquoise nails + chrome</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1t6zm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1e1t584</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>LynB Kitten Purrs 😺</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1t584</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1e1q976</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Sweet &amp; Simple :)</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oa4s1t1235cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1e1ste8</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>ILNP-Poison x My Private Rainbow X</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1ste8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1e1sp0p</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>ILNP Melody: A surprise favorite!</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1sp0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1e1rkwp</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Beginner tips</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e1rkwp/beginner_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1e1rhvz</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Decanted my new Mooncat polishes into empty (safe) bottles</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1rhvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1e1qsc6</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Orly Vintage</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jumjmpp275cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1e1qrcy</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Encounter The Bloom worth it? </t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e1qrcy/encounter_the_bloom_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1e1qby1</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Favorite metallics?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgujzjdn35cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1e1peuy</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>A surprising one-coater (Obscure, Ethereal charity polish)</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1peuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1e1p6b8</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Amid the Insects’ Lulling Serenade</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1p6b8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1e1ouc1</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Mani with the new PPG collection from the infamous mooncat</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1ouc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1e1or9t</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Water transfer decals vs stamping plates</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e1or9t/water_transfer_decals_vs_stamping_plates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1e1oe5v</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Nail Lover Seeking Good Yellow Recs</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e1oe5v/nail_lover_seeking_good_yellow_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1e1o2sv</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Adding two bottles together</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e1o2sv/adding_two_bottles_together/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1e1nsqg</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Topcoat UV Blocking Capabilities &amp; Solar Polishes</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1nsqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1e1nqzj</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>♓️🐠this polish and i both have real big feelings🐠♓️</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1nqzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1e1mawi</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Very Valentino - Cirque Colors</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1mawi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1e1nafv</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Damaged nails after removing press ons, what should I do? Can I put some nail polish on to hide the "cracks"? </t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlq422zpg4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1e1n8tb</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Nail polish buys during UK trip?</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e1n8tb/nail_polish_buys_during_uk_trip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1e1n7zy</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Buying a setup for my partner</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e1n7zy/buying_a_setup_for_my_partner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1e1n1rm</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>She wore blue velvet 💙</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1n1rm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1e1mpb0</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Easy but fun: Nails like gems for summer!</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t35xnwzlc4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1e1mehm</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Amazed by Seche-VIVE</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1rku3pf9a4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1e1ltkc</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Bringing out the sparkly purple for a third date 💜✨</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7495j2w364cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1e1lj5y</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Someone's request lead me to a little mystery on this color</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1lj5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1e1liyj</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>What can I do to spice these up?</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cs55tsgy34cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1e1jz8h</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Layering experiment</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1jz8h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1e1jqv4</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glossy taco turns matte at nail tips? </t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ks04andwq3cd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1e1jgc2</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Rip my beautiful nails</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxmlvkzoo3cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1e1isbe</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Summer sprinkles</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42ngpczhj3cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1e1imyf</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>90’s vibe set ahead of a festival tomorrow!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knxw96qci3cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1e1hi5r</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Ashwaganda and Nails</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e1hi5r/ashwaganda_and_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1e1hdqd</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Where to find original OPI nail envy?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e1hdqd/where_to_find_original_opi_nail_envy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1e1hc1c</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Do my hands look off with short nails? I had to cut them :(</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1hc1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1e1gigs</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Another one worth the hype!</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1gigs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1e1g9ie</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Cherry Nails! 🍒</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxjkoftky2cd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1e1dxh9</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Looking for a gold chrome top coat</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1dxh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1e1zw40</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Do you think this design is pretty?</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1zw40</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1e1y4ar</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>newest set!! (from a new member here :D)</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1y4ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1e1u7c8</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>In what occasion would you wear this set?</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1u7c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1e1skya</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Summer nails 💅</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4eyruglk5cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1e1qtqp</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Snake nestled in some flowers </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1qtqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1e1qsq9</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Matchy-matchy!</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1qsq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1e1qr4t</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Nail Picture help</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e1qr4t/nail_picture_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1e1ps1g</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Koi fish nails!!</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdc4unzgz4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1e1plwh</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Diy fiesta nails </t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e1plwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1e1o0l2</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aurora Gel X nails @ornellas_nails on IG. </t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4seh5n4bm4cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1e1lr4o</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Love my nails💖💖💖</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gogvg0rl54cd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1e1loxr</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Ready for the Bling-end lol</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/libcaab654cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1e1jcg4</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>3D chrome lines with gems?</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yvym8eqtn3cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1e1cm9c</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Beginner nail artist :) did this come out okay?</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y0xrfbku1cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jul 14 08:10:21 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_07_14.xlsx
+++ b/data/2024_07_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1168"/>
+  <dimension ref="A1:C1353"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20289,6 +20289,3151 @@
         </is>
       </c>
     </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1e2wxxm</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>I hardly ever get mine done.  Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2wxxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1e2wo2i</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Feeling like a Chocolate milkshake</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jy7z73gvfcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1e2w8zr</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Magnetic Ombre for Maid of Honor❤️</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jn4nwopdqfcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1e2vmum</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>First time doing 3D Nails🥹</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2vmum</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1e2v8sv</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Sunset Ombré Nails!</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2v8sv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1e2uspz</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>what do u think?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ge75zcr9fcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1e2ucck</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Nakey nails</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2ucck</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1e2tpjx</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Which do you like best glossy or matte?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4lula37sxecd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1e2snp7</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Which shape looks best?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2snp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1e2s8sr</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>My villain nails</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awsyf85siecd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1e2s1pc</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92aaejbvgecd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1e2s15d</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feelin Barbie classic today and lovin it. </t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfro9qrpgecd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1e2r2ie</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Sparkling lime 🍋‍🟩 ✨</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2r2ie</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1e2qs1x</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>How much do you rate my manicure from 1 to 10?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nusinh8r4ecd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1e2qohl</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>What color should I try next?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2qohl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1e2qoc3</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Best velvet/magnetic style press-on nails?</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e2qoc3/best_velvetmagnetic_style_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1e2qhli</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Just got my wedding press ons taken off a few weeks ago… what does it mean?</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7q078dbx1ecd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1e2q3yq</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Shaping nails before applying?</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvfc0ny8ydcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1e2q3qq</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Nail lifting help</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1t74df6ydcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1e2pbgz</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Birthday nail help!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2pbgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1e2paaa</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>space nails with progressively more cursed poses</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2paaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1e2ptl1</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>How do I get rid of this dark skin?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2ptl1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1e2prn1</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting nail art </t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2prn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1e2pfu3</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Feeling cute, first regular polish manicure in forever.</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25x6xv7vrdcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1e2p8d9</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>got my nails done</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2p8d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1e2p1cc</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>first set</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9ocle19odcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1e2ov8x</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Blooming Gel</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4oa0vlpmdcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1e2g6sv</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>how much would u pay for these?</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yz3bogb4pbcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1e2iytl</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Help with splitting nail</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e2iytl/help_with_splitting_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1e2mr7z</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>My First Manicure</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2mr7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1e2ogn8</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Clownin’ around 🤡</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kuav115jdcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1e2ofnn</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>before and after</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2ofnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1e2oadb</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>💙💙💙</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pkknbavnhdcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1e2o7rr</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>White Nails 🤍</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2o7rr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1e2nxr1</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>🦈duh dun, duh dun🦈 Shark Week!</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2nxr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1e2nn7m</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Dry paste for Japanese manicure</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e2nn7m/dry_paste_for_japanese_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1e2n7fh</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>bought some new gels</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dxmbp0i8dcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1e2ms0z</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Photo inspired and made by my friend @sheila_villagra_nails</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hawedai35dcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1e2mr8o</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love a French tip 💅 </t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kiba9p1x4dcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1e2mjw8</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>this is my first time properly doing my nails, i pushed back the cuticle but there’s still a flap of skin. should i cut it or leave it?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwro7ekc3dcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1e2mhbv</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>any tips to stop biting my nails?</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7gwox7s2dcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1e2mf71</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CONTACT SOLUTION AFFECTING PRESS ONS </t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aguzug6b2dcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1e2mcx1</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Beach days make for the best nail backgrounds</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q1blnrts1dcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1e2m6qg</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqutsktf0dcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1e2jofa</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mermaid Nail Collection </t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghp1srhegccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1e2gzv9</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>HELP GEL X AND BLISTER???</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frnwg0qcvbcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1e2gxwg</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>How do you swatch magnetics?</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e2gxwg/how_do_you_swatch_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1e2ehij</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>My latest summer diy press-on set! 🫐🦋🥏</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2ehij</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1e2e33l</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>How do you guys find good nail techs/salons?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e2e33l/how_do_you_guys_find_good_nail_techssalons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1e2cpva</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>I have to get these nails off!!</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e2cpva/i_have_to_get_these_nails_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1e2bs6x</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>2 weeks of growth !! (Credit to Jenny @jandj_nailspa on insta)</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y3o4131racd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1e2aurr</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Help - Nails breaking vertically</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2aurr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1e27kze</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How soon after a fungal nail can I get acrylics? </t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e27kze/how_soon_after_a_fungal_nail_can_i_get_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1e26kdn</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Magneta nails collection</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e26kdn/magneta_nails_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1e26hdj</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Maintenance </t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e26hdj/nail_maintenance/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1e25ocw</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Good or bad LED Lamp?</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e25ocw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1e2lkg7</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>What type of nails do I have/how to make them look better</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2ty0jujvccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1e2ljru</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh paint job </t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2ljru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1e2ldyy</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Hiiiii I’m Kellie and I love stamping!</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2ldyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1e2l5yj</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Nail art ideas</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ar7rmvcsccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1e2kq1g</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Can I put regular nail polish over rubber base gel?</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e2kq1g/can_i_put_regular_nail_polish_over_rubber_base_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1e2klfw</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Polish and Beauty Expo bound</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8l43lccrnccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1e2kj63</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>How did my new nail tech do?</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2kj63</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1e2kf3b</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Second set</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2kf3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1e2kc6w</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Hello, How many days to wait to get your nails done again?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lztiid9plccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1e2k3nl</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>New nails, decided to try square I stead of my usual rounded</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0uxsaesjccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1e2jum6</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Blush Pink 🩷</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2jum6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1e2joa6</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>In love with red jelly polish</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eab6krjcgccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1e2jlvc</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Lavender Ribbon nails 🙃</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2jlvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1e2jjc0</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Disney nails!</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iblp30o9fccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1e2j9dt</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Natural nails did a jelly polish with glitter accent nails. What do we think? ☺️</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2j9dt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1e2j548</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Long or short ?</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2j548</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1e2j537</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>First time doing my own nails (gel). Be honest with me- Do they look terrible?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2j537</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1e2ivpb</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Iso unpaid Recommendations </t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e2ivpb/iso_unpaid_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1e2irms</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Does one ever go wrong with butterflies and pearls? 🦋</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z77hesa59ccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1e2im6u</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>new set</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2im6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1e2iglz</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Felt like a summer whirlpool</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2iglz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1e2icny</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>are these funky weird</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2icny</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1e2hyzu</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh squeezed 🍋 🩵 </t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8bjnrv03ccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1e2gtaa</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Fresh Set! More feminine than I usually go, but I love it!</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wg8kq3uwtbcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1e2ghie</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Would you believe me if I told you this match was an accident?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7s6rzxerbcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1e2ggxs</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>It was time to give love to my hands</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9in6zx5brbcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1e2g59a</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>first time!</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2g59a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1e2fw7g</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Sparkling Pink dip with Chrome French</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2fw7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1e2fd0h</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Nail glue recommendations/retention issues</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1e2fd0h/nail_glue_recommendationsretention_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1e2erwh</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>New nails 🩵🌊🧜🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4gt4t4debcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1e2eiuq</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Latest Mani 💅 </t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2eiuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1e2efww</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>bubbly polish/peeling?</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2efww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1e2e2e6</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>So soooo happy.</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2e2e6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1e2dxfd</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>This is the closest I’ll get to having Ultraviolet nails using regular polish!</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2dxfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1e2djb2</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>My first set. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vmw80wt4bcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1e2dg6v</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>orange girl !</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zo6be5l54bcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1e2db83</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>A little out of my comfort zone color wise but I do love them</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2db83</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1e2d5yn</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Recs for GEL prugly colors?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2d5yn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1e2cncw</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Cosmic Nails</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2cncw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1e2c3cy</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried someone new today and let them do whatever they wanted. Pretty pleased with the outcome </t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/059u2gaktacd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1e2c25z</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s cold and rainy in the UK so I treated myself to some summery nails! They remind me of cupcake icing 🧁 </t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2c25z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1e2c0vv</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>First time doing acrylics</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2c0vv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1e2bn6n</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>🧿🪬</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cl8ddyawpacd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1e2bkoi</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>How can I improve my gel skills?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2bkoi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1e2wx3k</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Feedback on almond shape</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2wx3k/feedback_on_almond_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1e2wbzx</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>2nd set on myself - mermaid treasure nails!</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nam2s47krfcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1e2vdat</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Allergic to regular nail polish?</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2vdat/allergic_to_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1e2vco1</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Does anyone make a cool purple base with a cool pink shimmer polish?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2vco1/does_anyone_make_a_cool_purple_base_with_a_cool/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1e2v92a</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Does anyone make a dark blue polish with a yellow shimmer for like stars or city lights vibes?</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2v92a/does_anyone_make_a_dark_blue_polish_with_a_yellow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1e2tzlb</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Base/Too Coats and Nail Chemistry</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2tzlb/basetoo_coats_and_nail_chemistry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1e2swi3</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Having issues with the Emily De Molly peel off base coat</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2swi3/having_issues_with_the_emily_de_molly_peel_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1e2rzj8</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>🐸 ✨</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2rzj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1e2rwrh</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>My first ever attempt at checkerboard nails!</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2rwrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1e2rlk4</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Im... obsessed with this neon red orange. Dupes?</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xd0jhblpcecd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1e2r6ji</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>LF&gt; Dupe of Mooncat's "Don't cry bubbles" without the big glitters</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2r6ji/lf_dupe_of_mooncats_dont_cry_bubbles_without_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1e2qzjj</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Dreamt about a jelly sandwich today.</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2qzjj/dreamt_about_a_jelly_sandwich_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1e2qkdw</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>my favorite neutral 🩰</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcukn3mo2ecd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1e2pkxc</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Moonjelly 🌙✨</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tp021f8tdcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1e2o992</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Remove stubborn builder gel</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2o992/remove_stubborn_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1e2p4z4</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why does matte polish crack so bad? </t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1b4bfnr4pdcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1e2ouw3</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Spooky summer</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2ouw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1e2omui</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Sun-kissed Dark Horse 🌅🐎</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2omui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1e2n46h</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Sunset Nails at Sunset</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ea1hnnq7dcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1e2n2n3</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>See You Space Cowboy - I Can't Stop Staring</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qahgmo2d7dcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1e2mium</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>You'll have to imagine the clown meme, applying more clown makeup. That's me buying polish apparently.</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2mium</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1e2ljm4</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Shinobu - Pahlish June 24 PPU</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2ljm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1e2l8c0</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Man….nude nails are so hard to capture on camera. Hope I did this colour justice!</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04lg0wkwsccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1e2l3yc</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>King’s Gambit</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2l3yc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1e2kh9g</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art </t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2kh9g/nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1e2jymr</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>The purple of my dreams</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c6vshvxniccd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1e2jyxf</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Neato Mojito Sassy Sauce!</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2jyxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1e2jpao</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Paid $30 to have my nails done at a Esthetics school. How can I fix them from home?</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbo3i6jlgccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1e2j2zp</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Something seems wrong with my Royal Crush from Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2j2zp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1e2j08d</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>An Electric Eel in Love</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2j08d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1e2iv52</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>How do I get this vibe but matching my skin tone?</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2iv52</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1e2ip3g</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>First time making nail vinyls with my cricut, I think it’s a success.</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9jkgxdl8ccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1e2i0hb</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Morus Alba, My Foe</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2i0hb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1e2hpyv</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Love a mini haul moment</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2hpyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1e2hhe9</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Mooncat Mermaid Bait 🩵</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14e2aqm8zbcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1e2hdqp</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>favorite off-white shades?</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2hdqp/favorite_offwhite_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1e2h8uw</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First neon polishes! </t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2h8uw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1e2gv7x</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Update - Solar Polish/Topcoat Experiment Part 2 + 3</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9kw0x2aubcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1e2ggex</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Opinions on Colores de Carol</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2ggex/opinions_on_colores_de_carol/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1e2g0b2</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Popsicle Nails 🍓🍊</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2g0b2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1e2frlq</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Bitten is one of my new favorites 😍🩸</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2frlq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1e2f34z</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Latte Cloud vibes 🌟☁️</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2f34z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1e2evlu</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>First time getting my nails done in over a year and I love them 💖</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27fim0w4fbcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1e2e6n3</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Some bobs burger nails I have created 🥰 my fav show ever and had to give Louise the ketchup since she hates mustard 😞</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r2mg5zes9bcd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1e2e5h2</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Need Help with shaping my natural nails so they stop looking like this / make my nails beds look less wide ?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p55np3mj9bcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1e2e1nf</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>🩷🍦Ice Cream🍦💛</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2e1nf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1e2ds49</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Appreciation post: Glisten and Glow ridge filler is the one 🙏</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2ds49</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1e2doaj</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Waves or clouds</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2doaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1e2d9xf</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>"we have polish at home"</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2d9xf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1e2d38o</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Neon Dinosaur Footprints</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2d38o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1e2cjwf</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>current essie combo!</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2cjwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1e2c0k7</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Brands that do Thermals/fav thermals? 🔥❄️</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e2c0k7/brands_that_do_thermalsfav_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1e2b555</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Garden Path</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2b555</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1e24k39</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Summer nails (feat. Cirque Saffron Jelly and Deco Miami stickers)</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clfnhrxzm8cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1e24qt9</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Is this OPI polish real or fake?</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e24qt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1e28ig5</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Rainbow Flakies! (polish details in comment)</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e28ig5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1e28amh</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Nailpolish and Data obsession you say? Nahh</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1e28amh/nailpolish_and_data_obsession_you_say_nahh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1e2815m</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is Caelid! </t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qszzzx8fs9cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1e2s1t3</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Green nails! 💚</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2s1t3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1e2q2zl</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I never made goth/alternative nails before are these okay? They are for a friend :) </t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2q2zl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1e2p0e9</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>My nails❤️</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xbv8mw0odcd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1e2oqz5</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Pink for Laura</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szx2xllmldcd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1e2o380</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Nails 8</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hd71e5oufdcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1e2mhui</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Is it better to just invest in the pricier, better brushes?</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1e2mhui/is_it_better_to_just_invest_in_the_pricier_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1e2ler3</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Love is in the Air! I love youuuu...</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9shxiibuccd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1e2l099</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Went a little extra to head to the Polish and Beauty Expo tomorrow</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gb7l5713rccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1e2kut3</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Coastal cowgirl 🤠🐚</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2kut3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1e2ktvv</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Nail art ideas Please</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kx7htw0opccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1e2jk1o</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Disney nails!</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rxfnuaffccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1e2ipd8</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lone giraffe </t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2ipd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1e2icaw</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Summer vibes</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3jfqfus5ccd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1e2hx4e</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">beautiful design and beautiful colors ❤️ </t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2hx4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1e2hb69</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>My first nail “job”!</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bt427bxuxbcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1e2h7w6</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Winter nails 🖤</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrxvj1z4xbcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1e2gwgm</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>New listing</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2mhzoylubcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1e2gotw</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Bojack Nails</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2gotw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1e2fmrh</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>I asked my nail tech to match my roller skates, and she CRUSHED it!! (Nails by @dime_out on IG❤️)</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2fmrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1e2dkmu</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>nail pics hitting different since getting engaged</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2dkmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1e2dgwy</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Pirate’s Treasure Nails</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5ar7k5b4bcd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1e2d2fs</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Summer Nails - Candy Green Apple 🍭🍏</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2d2fs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1e2cugs</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>My Bee-utiful gnome set I hand painted</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4eo3x9jzacd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1e2b171</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Ice cream dessert set</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e2b171</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1e29m7o</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Where would you wear these? Personally to a Ren fair.</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e29m7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1e29fpk</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>mini paintbrush for the win 🕺</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1e29fpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1e28n21</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>🍒🍒</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tt199nzy9cd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>